<commit_message>
signoutworks and buttonsgrey out
</commit_message>
<xml_diff>
--- a/public/excel/data_streamer.xlsx
+++ b/public/excel/data_streamer.xlsx
@@ -191,7 +191,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -211,6 +211,12 @@
       <sz val="16"/>
       <color rgb="FF696969"/>
       <name val="Segoe UI Light"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
@@ -273,12 +279,6 @@
       <sz val="13"/>
       <color rgb="FF505050"/>
       <name val="Segoe UI"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -671,72 +671,75 @@
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="7" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="8" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="8" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="7" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="9" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="10" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="10" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="10" applyFont="1" fillId="6" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="10" applyFont="1" fillId="6" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="11" applyFont="1" fillId="6" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="10" applyFont="1" fillId="6" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="6" applyBorder="1" fontId="10" applyFont="1" fillId="6" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="7" applyBorder="1" fontId="11" applyFont="1" fillId="6" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="8" applyBorder="1" fontId="7" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="9" applyBorder="1" fontId="10" applyFont="1" fillId="6" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="10" applyBorder="1" fontId="10" applyFont="1" fillId="6" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="11" applyBorder="1" fontId="11" applyFont="1" fillId="6" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="6" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="7" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="7" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="6" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="8" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="9" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="9" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="9" applyFont="1" fillId="6" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="9" applyFont="1" fillId="6" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="10" applyFont="1" fillId="6" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="9" applyFont="1" fillId="6" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="6" applyBorder="1" fontId="9" applyFont="1" fillId="6" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="7" applyBorder="1" fontId="10" applyFont="1" fillId="6" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="8" applyBorder="1" fontId="6" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="9" applyBorder="1" fontId="9" applyFont="1" fillId="6" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="10" applyBorder="1" fontId="9" applyFont="1" fillId="6" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="11" applyBorder="1" fontId="10" applyFont="1" fillId="6" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="7" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -758,19 +761,19 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="7" applyFont="1" fillId="7" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="11" applyFont="1" fillId="7" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="12" applyBorder="1" fontId="9" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="12" applyFont="1" fillId="7" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="8" applyFont="1" fillId="7" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="12" applyFont="1" fillId="7" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="12" applyBorder="1" fontId="10" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="13" applyFont="1" fillId="7" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="12" applyFont="1" fillId="7" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="13" applyFont="1" fillId="7" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -778,9 +781,6 @@
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -794,13 +794,13 @@
     <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="13" applyBorder="1" fontId="13" applyFont="1" fillId="8" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="13" applyBorder="1" fontId="14" applyFont="1" fillId="8" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="14" applyBorder="1" fontId="13" applyFont="1" fillId="8" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="14" applyBorder="1" fontId="14" applyFont="1" fillId="8" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="15" applyBorder="1" fontId="14" applyFont="1" fillId="9" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="15" applyBorder="1" fontId="15" applyFont="1" fillId="9" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -812,59 +812,59 @@
     <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="15" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="15" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="8" applyFont="1" fillId="10" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="16" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="16" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="9" applyFont="1" fillId="10" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="8" applyFont="1" fillId="10" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="9" applyFont="1" fillId="10" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="16" applyBorder="1" fontId="14" applyFont="1" fillId="11" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="16" applyBorder="1" fontId="14" applyFont="1" fillId="11" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="16" applyBorder="1" fontId="15" applyFont="1" fillId="11" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="16" applyBorder="1" fontId="15" applyFont="1" fillId="11" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="17" applyBorder="1" fontId="15" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="17" applyBorder="1" fontId="15" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="18" applyBorder="1" fontId="14" applyFont="1" fillId="12" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="18" applyBorder="1" fontId="14" applyFont="1" fillId="12" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="17" applyBorder="1" fontId="16" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="17" applyBorder="1" fontId="16" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="18" applyBorder="1" fontId="15" applyFont="1" fillId="12" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="18" applyBorder="1" fontId="15" applyFont="1" fillId="12" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="19" applyBorder="1" fontId="14" applyFont="1" fillId="12" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="19" applyBorder="1" fontId="14" applyFont="1" fillId="12" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="19" applyBorder="1" fontId="15" applyFont="1" fillId="12" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="19" applyBorder="1" fontId="15" applyFont="1" fillId="12" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="19" applyBorder="1" fontId="14" applyFont="1" fillId="13" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="19" applyBorder="1" fontId="14" applyFont="1" fillId="13" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="19" applyBorder="1" fontId="15" applyFont="1" fillId="13" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="19" applyBorder="1" fontId="15" applyFont="1" fillId="13" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="16" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -881,8 +881,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A7:K22" displayName="TBL_HST" name="TBL_HST" id="1" totalsRowShown="0">
-  <autoFilter ref="A7:K22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A4:K5" displayName="TBL_CUR" name="TBL_CUR" id="1" totalsRowShown="0">
+  <autoFilter ref="A4:K5">
     <filterColumn hiddenButton="1" colId="0"/>
     <filterColumn hiddenButton="1" colId="1"/>
     <filterColumn hiddenButton="1" colId="2"/>
@@ -913,8 +913,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A4:K5" displayName="TBL_CUR" name="TBL_CUR" id="2" totalsRowShown="0">
-  <autoFilter ref="A4:K5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A7:K22" displayName="TBL_HST" name="TBL_HST" id="2" totalsRowShown="0">
+  <autoFilter ref="A7:K22">
     <filterColumn hiddenButton="1" colId="0"/>
     <filterColumn hiddenButton="1" colId="1"/>
     <filterColumn hiddenButton="1" colId="2"/>
@@ -1254,7 +1254,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="75" width="14.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="45" width="10.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="46" width="10.719285714285713" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="31" width="10.719285714285713" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="31" width="10.719285714285713" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="31" width="10.719285714285713" customWidth="1" bestFit="1"/>
@@ -1266,7 +1266,7 @@
     <col min="11" max="11" style="31" width="10.719285714285713" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="29.25">
       <c r="A1" s="56" t="s">
         <v>34</v>
       </c>
@@ -1281,7 +1281,7 @@
       <c r="J1" s="2"/>
       <c r="K1" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25" customFormat="1" s="6">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75" customFormat="1" s="6">
       <c r="A2" s="57" t="s">
         <v>35</v>
       </c>
@@ -1296,7 +1296,7 @@
       <c r="J2" s="7"/>
       <c r="K2" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="33.45">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="20.25">
       <c r="A3" s="58" t="s">
         <v>36</v>
       </c>
@@ -1363,7 +1363,7 @@
       <c r="J5" s="63"/>
       <c r="K5" s="63"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="21.75">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="21">
       <c r="A6" s="64" t="s">
         <v>39</v>
       </c>
@@ -1838,133 +1838,133 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="45" width="30.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="46" width="0.2907142857142857" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="46" width="30.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="47" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="47" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="46" width="30.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="47" width="0.2907142857142857" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="47" width="30.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="30" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="30" width="12.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="49.95000000000001" customFormat="1" s="6">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="4.5">
-      <c r="A3" s="38"/>
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
+      <c r="A3" s="39"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="24">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="41" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="41">
+      <c r="B4" s="42">
         <v>150</v>
       </c>
-      <c r="C4" s="42">
+      <c r="C4" s="43">
         <v>150</v>
       </c>
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="4.5">
-      <c r="A5" s="38"/>
-      <c r="B5" s="39"/>
-      <c r="C5" s="39"/>
+      <c r="A5" s="39"/>
+      <c r="B5" s="40"/>
+      <c r="C5" s="40"/>
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="24">
-      <c r="A6" s="40" t="s">
+      <c r="A6" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="41">
+      <c r="B6" s="42">
         <v>15</v>
       </c>
-      <c r="C6" s="42">
+      <c r="C6" s="43">
         <v>15</v>
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="4.5">
-      <c r="A7" s="38"/>
-      <c r="B7" s="39"/>
-      <c r="C7" s="39"/>
+      <c r="A7" s="39"/>
+      <c r="B7" s="40"/>
+      <c r="C7" s="40"/>
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="24">
-      <c r="A8" s="40" t="s">
+      <c r="A8" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="41">
+      <c r="B8" s="42">
         <v>10</v>
       </c>
-      <c r="C8" s="42">
+      <c r="C8" s="43">
         <v>10</v>
       </c>
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="4.5">
-      <c r="A9" s="38"/>
-      <c r="B9" s="39"/>
-      <c r="C9" s="39"/>
+      <c r="A9" s="39"/>
+      <c r="B9" s="40"/>
+      <c r="C9" s="40"/>
       <c r="D9" s="8"/>
       <c r="E9" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="24">
-      <c r="A10" s="40" t="s">
+      <c r="A10" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="41" t="s">
+      <c r="B10" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="42" t="s">
+      <c r="C10" s="43" t="s">
         <v>30</v>
       </c>
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="17.25">
-      <c r="A11" s="38"/>
-      <c r="B11" s="39"/>
-      <c r="C11" s="39"/>
+      <c r="A11" s="39"/>
+      <c r="B11" s="40"/>
+      <c r="C11" s="40"/>
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="17.25">
-      <c r="A12" s="38"/>
-      <c r="B12" s="39"/>
-      <c r="C12" s="39"/>
+      <c r="A12" s="39"/>
+      <c r="B12" s="40"/>
+      <c r="C12" s="40"/>
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="49.95000000000001" customFormat="1" s="6">
-      <c r="A13" s="43" t="s">
+      <c r="A13" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="44"/>
-      <c r="C13" s="44"/>
-      <c r="D13" s="43"/>
-      <c r="E13" s="43"/>
+      <c r="B13" s="45"/>
+      <c r="C13" s="45"/>
+      <c r="D13" s="44"/>
+      <c r="E13" s="44"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1998,7 +1998,7 @@
     <col min="9" max="9" style="32" width="16.719285714285714" customWidth="1" bestFit="1"/>
     <col min="10" max="10" style="31" width="60.71928571428572" customWidth="1" bestFit="1"/>
     <col min="11" max="11" style="32" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="30" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="33" width="12.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">

</xml_diff>